<commit_message>
Ajout couleur peau à questions pilot
</commit_message>
<xml_diff>
--- a/Users/Camille/Dropbox/Academique/Projets/BAV/questionsWording/questionsWording_BAV.xlsx
+++ b/Users/Camille/Dropbox/Academique/Projets/BAV/questionsWording/questionsWording_BAV.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="327">
   <si>
     <t>Are you?</t>
   </si>
@@ -155,24 +155,6 @@
     <t>Please type your age.</t>
   </si>
   <si>
-    <t>skinColorA</t>
-  </si>
-  <si>
-    <t>skinColorB</t>
-  </si>
-  <si>
-    <t>skinColorC</t>
-  </si>
-  <si>
-    <t>skinColorD</t>
-  </si>
-  <si>
-    <t>skinColorE</t>
-  </si>
-  <si>
-    <t>skinColorF</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -1014,6 +996,24 @@
   </si>
   <si>
     <t xml:space="preserve">Autre </t>
+  </si>
+  <si>
+    <t>#FFFFFF</t>
+  </si>
+  <si>
+    <t>#FFECCB</t>
+  </si>
+  <si>
+    <t>#ECCD73</t>
+  </si>
+  <si>
+    <t>#DAA605</t>
+  </si>
+  <si>
+    <t>#97754D</t>
+  </si>
+  <si>
+    <t>#723905</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1088,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1097,6 +1097,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -1416,7 +1417,7 @@
   <dimension ref="A1:D154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D5" sqref="D5:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1429,16 +1430,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1446,13 +1447,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1463,77 +1464,95 @@
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>174</v>
+      <c r="B4" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>175</v>
+      <c r="B5" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>321</v>
+      </c>
+      <c r="D5" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="6"/>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>322</v>
+      </c>
+      <c r="D6" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>42</v>
+      <c r="B7" s="6"/>
+      <c r="C7" t="s">
+        <v>323</v>
+      </c>
+      <c r="D7" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>43</v>
+      <c r="B8" s="6"/>
+      <c r="C8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D8" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
-        <v>44</v>
+      <c r="B9" s="6"/>
+      <c r="C9" t="s">
+        <v>325</v>
+      </c>
+      <c r="D9" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>45</v>
+      <c r="B10" s="6"/>
+      <c r="C10" t="s">
+        <v>326</v>
+      </c>
+      <c r="D10" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1541,13 +1560,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1555,10 +1574,10 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1566,10 +1585,10 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1577,13 +1596,13 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1591,10 +1610,10 @@
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1602,10 +1621,10 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1613,10 +1632,10 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1624,10 +1643,10 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1635,13 +1654,13 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1649,10 +1668,10 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1660,10 +1679,10 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1671,10 +1690,10 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1682,13 +1701,13 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1696,10 +1715,10 @@
         <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1707,13 +1726,13 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1721,10 +1740,10 @@
         <v>8</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1732,10 +1751,10 @@
         <v>8</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1743,13 +1762,13 @@
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D28" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1757,13 +1776,13 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D29" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1771,13 +1790,13 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D30" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1785,10 +1804,10 @@
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D31" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1796,10 +1815,10 @@
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1807,10 +1826,10 @@
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D33" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1818,13 +1837,13 @@
         <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D34" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1832,10 +1851,10 @@
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1843,10 +1862,10 @@
         <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D36" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1854,13 +1873,13 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D37" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1868,7 +1887,7 @@
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1876,7 +1895,7 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1884,13 +1903,13 @@
         <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D40" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1898,10 +1917,10 @@
         <v>14</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D41" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1909,10 +1928,10 @@
         <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D42" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1920,10 +1939,10 @@
         <v>14</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D43" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1931,10 +1950,10 @@
         <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1942,13 +1961,13 @@
         <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D45" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1956,10 +1975,10 @@
         <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1967,10 +1986,10 @@
         <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D47" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1978,10 +1997,10 @@
         <v>15</v>
       </c>
       <c r="C48" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D48" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1989,10 +2008,10 @@
         <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D49" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -2000,10 +2019,10 @@
         <v>15</v>
       </c>
       <c r="C50" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -2011,10 +2030,10 @@
         <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D51" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -2022,10 +2041,10 @@
         <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D52" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -2033,10 +2052,10 @@
         <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D53" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -2044,10 +2063,10 @@
         <v>15</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D54" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -2055,10 +2074,10 @@
         <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D55" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -2066,10 +2085,10 @@
         <v>15</v>
       </c>
       <c r="C56" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D56" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -2077,10 +2096,10 @@
         <v>15</v>
       </c>
       <c r="C57" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D57" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -2088,10 +2107,10 @@
         <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C58" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -2099,10 +2118,10 @@
         <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C59" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2110,13 +2129,13 @@
         <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C60" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D60" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2124,10 +2143,10 @@
         <v>18</v>
       </c>
       <c r="C61" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D61" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -2135,10 +2154,10 @@
         <v>18</v>
       </c>
       <c r="C62" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D62" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2146,13 +2165,13 @@
         <v>19</v>
       </c>
       <c r="B63" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C63" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D63" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -2160,10 +2179,10 @@
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D64" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2171,10 +2190,10 @@
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D65" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2182,10 +2201,10 @@
         <v>19</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D66" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
@@ -2193,13 +2212,13 @@
         <v>20</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C67" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D67" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
@@ -2208,10 +2227,10 @@
       </c>
       <c r="B68" s="3"/>
       <c r="C68" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D68" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
@@ -2220,10 +2239,10 @@
       </c>
       <c r="B69" s="3"/>
       <c r="C69" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D69" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
@@ -2232,10 +2251,10 @@
       </c>
       <c r="B70" s="3"/>
       <c r="C70" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D70" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
@@ -2244,10 +2263,10 @@
       </c>
       <c r="B71" s="3"/>
       <c r="C71" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D71" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
@@ -2256,10 +2275,10 @@
       </c>
       <c r="B72" s="3"/>
       <c r="C72" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D72" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -2267,13 +2286,13 @@
         <v>21</v>
       </c>
       <c r="B73" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C73" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D73" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2281,10 +2300,10 @@
         <v>21</v>
       </c>
       <c r="C74" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D74" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2292,10 +2311,10 @@
         <v>21</v>
       </c>
       <c r="C75" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D75" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -2303,10 +2322,10 @@
         <v>21</v>
       </c>
       <c r="C76" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D76" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -2314,10 +2333,10 @@
         <v>21</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D77" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2325,13 +2344,13 @@
         <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C78" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D78" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2339,10 +2358,10 @@
         <v>22</v>
       </c>
       <c r="C79" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D79" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2350,10 +2369,10 @@
         <v>22</v>
       </c>
       <c r="C80" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D80" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -2361,10 +2380,10 @@
         <v>22</v>
       </c>
       <c r="C81" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D81" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -2372,13 +2391,13 @@
         <v>23</v>
       </c>
       <c r="B82" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C82" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D82" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -2386,10 +2405,10 @@
         <v>23</v>
       </c>
       <c r="C83" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D83" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -2397,13 +2416,13 @@
         <v>24</v>
       </c>
       <c r="B84" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C84" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D84" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -2411,10 +2430,10 @@
         <v>24</v>
       </c>
       <c r="C85" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D85" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -2422,10 +2441,10 @@
         <v>24</v>
       </c>
       <c r="C86" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D86" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -2433,10 +2452,10 @@
         <v>24</v>
       </c>
       <c r="C87" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D87" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -2444,10 +2463,10 @@
         <v>24</v>
       </c>
       <c r="C88" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D88" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -2455,10 +2474,10 @@
         <v>24</v>
       </c>
       <c r="C89" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D89" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -2466,10 +2485,10 @@
         <v>24</v>
       </c>
       <c r="C90" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D90" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -2477,13 +2496,13 @@
         <v>25</v>
       </c>
       <c r="B91" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C91" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D91" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -2491,10 +2510,10 @@
         <v>25</v>
       </c>
       <c r="C92" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D92" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -2502,10 +2521,10 @@
         <v>25</v>
       </c>
       <c r="C93" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D93" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -2513,10 +2532,10 @@
         <v>25</v>
       </c>
       <c r="C94" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D94" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -2524,10 +2543,10 @@
         <v>25</v>
       </c>
       <c r="C95" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D95" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -2535,13 +2554,13 @@
         <v>26</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D96" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -2550,10 +2569,10 @@
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D97" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -2562,10 +2581,10 @@
       </c>
       <c r="B98" s="5"/>
       <c r="C98" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D98" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -2573,13 +2592,13 @@
         <v>27</v>
       </c>
       <c r="B99" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D99" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -2587,10 +2606,10 @@
         <v>27</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D100" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -2598,10 +2617,10 @@
         <v>27</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D101" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -2609,10 +2628,10 @@
         <v>27</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D102" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -2620,10 +2639,10 @@
         <v>27</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D103" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -2631,10 +2650,10 @@
         <v>27</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D104" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -2642,13 +2661,13 @@
         <v>28</v>
       </c>
       <c r="B105" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D105" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -2656,10 +2675,10 @@
         <v>28</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D106" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -2667,10 +2686,10 @@
         <v>28</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D107" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -2678,10 +2697,10 @@
         <v>28</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D108" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -2689,10 +2708,10 @@
         <v>28</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D109" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -2700,13 +2719,13 @@
         <v>29</v>
       </c>
       <c r="B110" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D110" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -2714,10 +2733,10 @@
         <v>29</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D111" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -2725,10 +2744,10 @@
         <v>29</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D112" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
@@ -2736,13 +2755,13 @@
         <v>30</v>
       </c>
       <c r="B113" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D113" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -2750,10 +2769,10 @@
         <v>30</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D114" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -2761,10 +2780,10 @@
         <v>30</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D115" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -2772,10 +2791,10 @@
         <v>30</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D116" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -2783,13 +2802,13 @@
         <v>31</v>
       </c>
       <c r="B117" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D117" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -2797,10 +2816,10 @@
         <v>31</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D118" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -2808,13 +2827,13 @@
         <v>32</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -2823,10 +2842,10 @@
       </c>
       <c r="B120" s="2"/>
       <c r="C120" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D120" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -2835,10 +2854,10 @@
       </c>
       <c r="B121" s="2"/>
       <c r="C121" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D121" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -2847,10 +2866,10 @@
       </c>
       <c r="B122" s="2"/>
       <c r="C122" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D122" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -2859,10 +2878,10 @@
       </c>
       <c r="B123" s="2"/>
       <c r="C123" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D123" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -2871,10 +2890,10 @@
       </c>
       <c r="B124" s="2"/>
       <c r="C124" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D124" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -2882,13 +2901,13 @@
         <v>33</v>
       </c>
       <c r="B125" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -2896,10 +2915,10 @@
         <v>33</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D126" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -2907,10 +2926,10 @@
         <v>33</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D127" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -2918,10 +2937,10 @@
         <v>33</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D128" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
@@ -2929,10 +2948,10 @@
         <v>33</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D129" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -2940,10 +2959,10 @@
         <v>33</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D130" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -2951,10 +2970,10 @@
         <v>33</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D131" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -2962,10 +2981,10 @@
         <v>33</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D132" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -2973,10 +2992,10 @@
         <v>33</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D133" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
@@ -2984,13 +3003,13 @@
         <v>34</v>
       </c>
       <c r="B134" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D134" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
@@ -2998,10 +3017,10 @@
         <v>34</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D135" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
@@ -3009,10 +3028,10 @@
         <v>34</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D136" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -3020,10 +3039,10 @@
         <v>34</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D137" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -3031,13 +3050,13 @@
         <v>35</v>
       </c>
       <c r="B138" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D138" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
@@ -3045,10 +3064,10 @@
         <v>35</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D139" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
@@ -3056,10 +3075,10 @@
         <v>35</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D140" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
@@ -3067,10 +3086,10 @@
         <v>35</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D141" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
@@ -3078,10 +3097,10 @@
         <v>35</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D142" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
@@ -3089,10 +3108,10 @@
         <v>35</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D143" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
@@ -3100,10 +3119,10 @@
         <v>35</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D144" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
@@ -3111,10 +3130,10 @@
         <v>35</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D145" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
@@ -3122,10 +3141,10 @@
         <v>35</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D146" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
@@ -3133,10 +3152,10 @@
         <v>35</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D147" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
@@ -3144,10 +3163,10 @@
         <v>35</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D148" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
@@ -3155,10 +3174,10 @@
         <v>35</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D149" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
@@ -3166,10 +3185,10 @@
         <v>35</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D150" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
@@ -3177,13 +3196,13 @@
         <v>36</v>
       </c>
       <c r="B151" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C151" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D151" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
@@ -3191,10 +3210,10 @@
         <v>36</v>
       </c>
       <c r="C152" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D152" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
@@ -3202,10 +3221,10 @@
         <v>36</v>
       </c>
       <c r="C153" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D153" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
@@ -3213,15 +3232,15 @@
         <v>36</v>
       </c>
       <c r="C154" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D154" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>